<commit_message>
import api create for import exercise data
</commit_message>
<xml_diff>
--- a/Workout_Exercise_Expanded_Database.xlsx
+++ b/Workout_Exercise_Expanded_Database.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DREAMWORLD\Desktop\coach_event\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Node\client-coach-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046E50C-F899-4AD3-B6D7-58F3F627B9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,24 +24,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Instructions (Text)</t>
-  </si>
-  <si>
-    <t>Instructions (Image URLs)</t>
-  </si>
-  <si>
-    <t>Instructions (Video URLs)</t>
-  </si>
-  <si>
-    <t>Muscle Groups Targeted</t>
-  </si>
-  <si>
-    <t>Equipment Required</t>
-  </si>
-  <si>
     <t>Push-Up</t>
   </si>
   <si>
@@ -332,12 +313,30 @@
   </si>
   <si>
     <t>3196293-uhd_3840_2160_25fps.mp4</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>muscleGroups</t>
+  </si>
+  <si>
+    <t>videoUrl</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,9 +425,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -466,9 +465,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -503,7 +502,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,7 +537,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -711,11 +710,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,527 +733,528 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G20" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D21" r:id="rId9" xr:uid="{E4515A17-BB71-4B7D-BD9E-2FB91D4D931F}"/>
-    <hyperlink ref="D18" r:id="rId10" xr:uid="{4736B4AE-73B6-4FAD-92FB-E4C54C633FFB}"/>
-    <hyperlink ref="D17" r:id="rId11" xr:uid="{AC24A08C-62AB-47BA-A833-C5269B86097A}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{ECFE6C26-103F-45B7-B3E8-14D864FB19D7}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{8EA97672-72E8-41E5-944E-5D70001CAD6B}"/>
-    <hyperlink ref="D13" r:id="rId14" xr:uid="{D66780B3-C619-415D-9922-170EDEE2A14F}"/>
-    <hyperlink ref="D12" r:id="rId15" xr:uid="{59B7E461-4670-4358-8A5B-F6CA6F31893C}"/>
-    <hyperlink ref="D11" r:id="rId16" xr:uid="{7BCE8603-7095-460D-B2D6-6AE901904DE1}"/>
-    <hyperlink ref="D8" r:id="rId17" xr:uid="{FFE7A02E-6A1F-4DBD-B208-389CFDC805B4}"/>
-    <hyperlink ref="D7" r:id="rId18" xr:uid="{1DA6D8B8-EA81-4E6F-BE8C-8AE0908DF109}"/>
-    <hyperlink ref="D5" r:id="rId19" xr:uid="{2C181D8E-3E91-41CC-87F8-FB7AB2E308E5}"/>
-    <hyperlink ref="D3" r:id="rId20" xr:uid="{65676318-160C-4186-B2B5-ED3D55CB8781}"/>
-    <hyperlink ref="E21" r:id="rId21" xr:uid="{D806DEC6-F66D-4CCE-BF83-4082CD0DB84E}"/>
-    <hyperlink ref="E20" r:id="rId22" xr:uid="{C780ACB9-7B93-4665-8C9B-9CE0728D9EFB}"/>
-    <hyperlink ref="E19" r:id="rId23" xr:uid="{9BB6A6E9-9486-4106-A422-E2CCE8D5839A}"/>
-    <hyperlink ref="E18" r:id="rId24" xr:uid="{7133824C-CD42-487D-9EAF-C3456C79130A}"/>
-    <hyperlink ref="E17" r:id="rId25" xr:uid="{6542286E-1AC6-42E4-BE3F-3B2968A4C640}"/>
-    <hyperlink ref="E16" r:id="rId26" xr:uid="{9844A83C-83D4-4FB5-8140-7C43F993C2C7}"/>
-    <hyperlink ref="E15" r:id="rId27" xr:uid="{A8B3F3C7-7204-4E08-8BE9-40CC7A2EF96C}"/>
-    <hyperlink ref="E14" r:id="rId28" xr:uid="{6AEB2F92-F1F8-41AE-BFD4-35A08E2541A8}"/>
-    <hyperlink ref="E13" r:id="rId29" xr:uid="{72368224-CD99-43EB-B136-10E7B6A5770C}"/>
-    <hyperlink ref="E12" r:id="rId30" xr:uid="{18302878-54B5-4597-876A-066A56B3EA7D}"/>
-    <hyperlink ref="E11" r:id="rId31" xr:uid="{FDD74813-DBCB-4A2A-A732-72FE5AA1E803}"/>
-    <hyperlink ref="E10" r:id="rId32" xr:uid="{632C1388-1F46-43BB-BFCD-681DE8BF94FF}"/>
-    <hyperlink ref="E9" r:id="rId33" xr:uid="{5064A679-962E-4F0F-8131-100BDBEDA2D4}"/>
-    <hyperlink ref="E8" r:id="rId34" xr:uid="{9DE75196-B7BA-46C9-9FD7-E96B1989F34E}"/>
-    <hyperlink ref="E7" r:id="rId35" xr:uid="{D22A65F1-5D56-4BDB-B9E3-3234C7979CC2}"/>
-    <hyperlink ref="E6" r:id="rId36" xr:uid="{96568F73-C6FE-4DD1-BFB9-99E0E17AA912}"/>
-    <hyperlink ref="E5" r:id="rId37" xr:uid="{4FC5D62D-3272-4D62-8DA1-29CBE1AEE5CB}"/>
-    <hyperlink ref="E4" r:id="rId38" xr:uid="{19502328-CEC7-4DFD-95A6-50E262C47FD2}"/>
-    <hyperlink ref="E3" r:id="rId39" xr:uid="{7EA4ADE6-8990-4380-8670-22388189589B}"/>
-    <hyperlink ref="E2" r:id="rId40" xr:uid="{A2B07403-0841-455C-AF11-620DDF480FF2}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D14" r:id="rId6"/>
+    <hyperlink ref="D19" r:id="rId7"/>
+    <hyperlink ref="D20" r:id="rId8"/>
+    <hyperlink ref="D21" r:id="rId9"/>
+    <hyperlink ref="D18" r:id="rId10"/>
+    <hyperlink ref="D17" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D13" r:id="rId14"/>
+    <hyperlink ref="D12" r:id="rId15"/>
+    <hyperlink ref="D11" r:id="rId16"/>
+    <hyperlink ref="D8" r:id="rId17"/>
+    <hyperlink ref="D7" r:id="rId18"/>
+    <hyperlink ref="D5" r:id="rId19"/>
+    <hyperlink ref="D3" r:id="rId20"/>
+    <hyperlink ref="E21" r:id="rId21"/>
+    <hyperlink ref="E20" r:id="rId22"/>
+    <hyperlink ref="E19" r:id="rId23"/>
+    <hyperlink ref="E18" r:id="rId24"/>
+    <hyperlink ref="E17" r:id="rId25"/>
+    <hyperlink ref="E16" r:id="rId26"/>
+    <hyperlink ref="E15" r:id="rId27"/>
+    <hyperlink ref="E14" r:id="rId28"/>
+    <hyperlink ref="E13" r:id="rId29"/>
+    <hyperlink ref="E12" r:id="rId30"/>
+    <hyperlink ref="E11" r:id="rId31"/>
+    <hyperlink ref="E10" r:id="rId32"/>
+    <hyperlink ref="E9" r:id="rId33"/>
+    <hyperlink ref="E8" r:id="rId34"/>
+    <hyperlink ref="E7" r:id="rId35"/>
+    <hyperlink ref="E6" r:id="rId36"/>
+    <hyperlink ref="E5" r:id="rId37"/>
+    <hyperlink ref="E4" r:id="rId38"/>
+    <hyperlink ref="E3" r:id="rId39"/>
+    <hyperlink ref="E2" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>